<commit_message>
finisch translating french and fix some italian and english translations
</commit_message>
<xml_diff>
--- a/fr/data_and_scripts/data/datasetLaws.xlsx
+++ b/fr/data_and_scripts/data/datasetLaws.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitch/Google Drive/Work/Assegno di Ricerca 2017_2018/[2017-09] SIEC - History of Administrative Detention/1. Material/Resources/Corrected Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amelia/Documents/GitHub/00_work/prototype-siec/fr/data_and_scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52079684-E450-064C-A6DD-1333B6ADD7AA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="17840" tabRatio="871"/>
+    <workbookView xWindow="2100" yWindow="460" windowWidth="25600" windowHeight="17840" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all law" sheetId="1" r:id="rId1"/>
@@ -2556,9 +2557,6 @@
     <t>TI012</t>
   </si>
   <si>
-    <t>Legge di applicazione della legge federale del 25 giugno 1976 che modifica il Codice civile svizzero</t>
-  </si>
-  <si>
     <t>UR001</t>
   </si>
   <si>
@@ -3234,16 +3232,19 @@
     <t>cantonal</t>
   </si>
   <si>
-    <t>federal</t>
-  </si>
-  <si>
     <t>intercantonal</t>
+  </si>
+  <si>
+    <t>Legge di applicazione della legge fédérale del 25 giugno 1976 che modifica il Codice civile svizzero</t>
+  </si>
+  <si>
+    <t>fédéral</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -3358,7 +3359,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Excel Built-in Normal" xfId="1"/>
+    <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3755,11 +3756,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IO358"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A354" workbookViewId="0">
-      <selection activeCell="C367" sqref="C367"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3774,31 +3775,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1059</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1060</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>1062</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>1061</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>1063</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>1064</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>1065</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="18" t="s">
         <v>1066</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>1067</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -3821,7 +3822,7 @@
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -3841,7 +3842,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -3864,7 +3865,7 @@
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -3887,7 +3888,7 @@
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -3912,7 +3913,7 @@
         <v>17</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -3937,7 +3938,7 @@
         <v>20</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -3962,7 +3963,7 @@
         <v>23</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -3987,7 +3988,7 @@
         <v>27</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -4012,7 +4013,7 @@
         <v>31</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -4032,7 +4033,7 @@
         <v>35</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="37.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4055,7 +4056,7 @@
         <v>31</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4078,7 +4079,7 @@
         <v>42</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4101,7 +4102,7 @@
         <v>46</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4121,7 +4122,7 @@
         <v>50</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4141,7 +4142,7 @@
         <v>3</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4164,7 +4165,7 @@
         <v>55</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4187,7 +4188,7 @@
         <v>58</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4207,7 +4208,7 @@
         <v>3</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4230,7 +4231,7 @@
         <v>31</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4250,7 +4251,7 @@
         <v>2</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -4270,7 +4271,7 @@
         <v>4</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4290,7 +4291,7 @@
         <v>2</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="118" x14ac:dyDescent="0.2">
@@ -4310,7 +4311,7 @@
         <v>13</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4330,7 +4331,7 @@
         <v>50</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4350,7 +4351,7 @@
         <v>1</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4370,7 +4371,7 @@
         <v>1</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4390,7 +4391,7 @@
         <v>35</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4410,7 +4411,7 @@
         <v>2</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4430,7 +4431,7 @@
         <v>83</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4450,7 +4451,7 @@
         <v>35</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4470,7 +4471,7 @@
         <v>35</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4490,7 +4491,7 @@
         <v>35</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4510,7 +4511,7 @@
         <v>13</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4530,7 +4531,7 @@
         <v>35</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4550,7 +4551,7 @@
         <v>2</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -4570,7 +4571,7 @@
         <v>4</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4593,7 +4594,7 @@
       </c>
       <c r="H38" s="13"/>
       <c r="I38" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="118" x14ac:dyDescent="0.2">
@@ -4616,7 +4617,7 @@
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4639,7 +4640,7 @@
       </c>
       <c r="H40" s="13"/>
       <c r="I40" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4662,7 +4663,7 @@
       </c>
       <c r="H41" s="13"/>
       <c r="I41" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -4685,7 +4686,7 @@
       </c>
       <c r="H42" s="13"/>
       <c r="I42" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4708,7 +4709,7 @@
       </c>
       <c r="H43" s="13"/>
       <c r="I43" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4731,7 +4732,7 @@
       </c>
       <c r="H44" s="13"/>
       <c r="I44" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4754,7 +4755,7 @@
       </c>
       <c r="H45" s="13"/>
       <c r="I45" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="118" x14ac:dyDescent="0.2">
@@ -4775,7 +4776,7 @@
       </c>
       <c r="H46" s="13"/>
       <c r="I46" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -4796,7 +4797,7 @@
       </c>
       <c r="H47" s="13"/>
       <c r="I47" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="118" x14ac:dyDescent="0.2">
@@ -4817,7 +4818,7 @@
       </c>
       <c r="H48" s="13"/>
       <c r="I48" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="144" x14ac:dyDescent="0.2">
@@ -4838,7 +4839,7 @@
       </c>
       <c r="H49" s="13"/>
       <c r="I49" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -4859,7 +4860,7 @@
       </c>
       <c r="H50" s="13"/>
       <c r="I50" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4881,7 +4882,7 @@
         <v>83</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -4903,7 +4904,7 @@
         <v>35</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4925,7 +4926,7 @@
         <v>83</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4947,7 +4948,7 @@
         <v>83</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4969,7 +4970,7 @@
         <v>83</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4991,7 +4992,7 @@
         <v>83</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5013,7 +5014,7 @@
         <v>83</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5040,7 +5041,7 @@
         <v>27</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -5063,7 +5064,7 @@
       </c>
       <c r="H59" s="8"/>
       <c r="I59" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5086,7 +5087,7 @@
       </c>
       <c r="H60" s="8"/>
       <c r="I60" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -5109,7 +5110,7 @@
       </c>
       <c r="H61" s="8"/>
       <c r="I61" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -5136,7 +5137,7 @@
         <v>177</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="118" x14ac:dyDescent="0.2">
@@ -5159,7 +5160,7 @@
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -5184,7 +5185,7 @@
       </c>
       <c r="H64" s="5"/>
       <c r="I64" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5209,7 +5210,7 @@
         <v>185</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -5232,7 +5233,7 @@
       </c>
       <c r="H66" s="5"/>
       <c r="I66" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5257,7 +5258,7 @@
         <v>191</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -5280,7 +5281,7 @@
       </c>
       <c r="H68" s="5"/>
       <c r="I68" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -5305,7 +5306,7 @@
         <v>197</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -5328,7 +5329,7 @@
       </c>
       <c r="H70" s="5"/>
       <c r="I70" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -5353,7 +5354,7 @@
         <v>204</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -5376,7 +5377,7 @@
       </c>
       <c r="H72" s="5"/>
       <c r="I72" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5399,7 +5400,7 @@
         <v>209</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5420,7 +5421,7 @@
       </c>
       <c r="H74" s="13"/>
       <c r="I74" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -5441,7 +5442,7 @@
       </c>
       <c r="H75" s="13"/>
       <c r="I75" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -5464,7 +5465,7 @@
         <v>216</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5485,7 +5486,7 @@
       </c>
       <c r="H77" s="13"/>
       <c r="I77" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5508,7 +5509,7 @@
         <v>221</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -5531,7 +5532,7 @@
         <v>224</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -5552,7 +5553,7 @@
       </c>
       <c r="H80" s="13"/>
       <c r="I80" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -5575,7 +5576,7 @@
       </c>
       <c r="H81" s="3"/>
       <c r="I81" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5598,7 +5599,7 @@
       </c>
       <c r="H82" s="3"/>
       <c r="I82" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5623,7 +5624,7 @@
         <v>237</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5648,7 +5649,7 @@
         <v>241</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -5673,7 +5674,7 @@
         <v>245</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -5698,7 +5699,7 @@
         <v>248</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5723,7 +5724,7 @@
         <v>252</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5748,7 +5749,7 @@
         <v>255</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5773,7 +5774,7 @@
         <v>259</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="118" x14ac:dyDescent="0.2">
@@ -5798,7 +5799,7 @@
         <v>263</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5821,7 +5822,7 @@
       </c>
       <c r="H91" s="5"/>
       <c r="I91" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5844,7 +5845,7 @@
       </c>
       <c r="H92" s="5"/>
       <c r="I92" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5869,7 +5870,7 @@
         <v>273</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -5889,7 +5890,7 @@
         <v>4</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5911,7 +5912,7 @@
         <v>83</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -5933,7 +5934,7 @@
         <v>83</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -5955,7 +5956,7 @@
         <v>35</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5977,7 +5978,7 @@
         <v>83</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5999,7 +6000,7 @@
         <v>83</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6021,7 +6022,7 @@
         <v>83</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -6043,7 +6044,7 @@
         <v>35</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6065,7 +6066,7 @@
         <v>13</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6087,7 +6088,7 @@
         <v>13</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6109,7 +6110,7 @@
         <v>35</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6131,7 +6132,7 @@
         <v>83</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6151,7 +6152,7 @@
         <v>1</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6171,7 +6172,7 @@
         <v>1</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -6194,7 +6195,7 @@
       </c>
       <c r="H108" s="3"/>
       <c r="I108" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6219,7 +6220,7 @@
         <v>323</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6242,7 +6243,7 @@
       </c>
       <c r="H110" s="8"/>
       <c r="I110" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6267,7 +6268,7 @@
         <v>330</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6292,7 +6293,7 @@
         <v>334</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -6317,7 +6318,7 @@
         <v>338</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6340,7 +6341,7 @@
       </c>
       <c r="H114" s="5"/>
       <c r="I114" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6363,7 +6364,7 @@
       </c>
       <c r="H115" s="5"/>
       <c r="I115" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6386,7 +6387,7 @@
       </c>
       <c r="H116" s="5"/>
       <c r="I116" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6411,7 +6412,7 @@
         <v>351</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -6434,7 +6435,7 @@
       </c>
       <c r="H118" s="5"/>
       <c r="I118" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -6459,7 +6460,7 @@
         <v>358</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6484,7 +6485,7 @@
         <v>362</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6507,7 +6508,7 @@
       </c>
       <c r="H121" s="5"/>
       <c r="I121" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -6532,7 +6533,7 @@
         <v>368</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6557,7 +6558,7 @@
         <v>371</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="124" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -6580,7 +6581,7 @@
       </c>
       <c r="H124" s="5"/>
       <c r="I124" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6605,7 +6606,7 @@
         <v>376</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6630,7 +6631,7 @@
         <v>379</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6655,7 +6656,7 @@
         <v>382</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -6680,7 +6681,7 @@
         <v>385</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6705,7 +6706,7 @@
         <v>388</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -6728,7 +6729,7 @@
       </c>
       <c r="H130" s="5"/>
       <c r="I130" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6753,7 +6754,7 @@
         <v>393</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -6778,7 +6779,7 @@
         <v>396</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6803,7 +6804,7 @@
         <v>399</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6826,7 +6827,7 @@
       </c>
       <c r="H134" s="8"/>
       <c r="I134" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6849,7 +6850,7 @@
       </c>
       <c r="H135" s="5"/>
       <c r="I135" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -6872,7 +6873,7 @@
       </c>
       <c r="H136" s="8"/>
       <c r="I136" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
@@ -6895,7 +6896,7 @@
       </c>
       <c r="H137" s="5"/>
       <c r="I137" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6918,7 +6919,7 @@
       </c>
       <c r="H138" s="5"/>
       <c r="I138" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -6941,7 +6942,7 @@
       </c>
       <c r="H139" s="5"/>
       <c r="I139" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -6964,7 +6965,7 @@
       </c>
       <c r="H140" s="8"/>
       <c r="I140" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="141" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -6987,7 +6988,7 @@
       </c>
       <c r="H141" s="8"/>
       <c r="I141" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7010,7 +7011,7 @@
       </c>
       <c r="H142" s="8"/>
       <c r="I142" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7033,7 +7034,7 @@
       </c>
       <c r="H143" s="8"/>
       <c r="I143" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7056,7 +7057,7 @@
       </c>
       <c r="H144" s="8"/>
       <c r="I144" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -7079,7 +7080,7 @@
       </c>
       <c r="H145" s="8"/>
       <c r="I145" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="146" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7102,7 +7103,7 @@
       </c>
       <c r="H146" s="5"/>
       <c r="I146" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7125,7 +7126,7 @@
       </c>
       <c r="H147" s="5"/>
       <c r="I147" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7148,7 +7149,7 @@
       </c>
       <c r="H148" s="5"/>
       <c r="I148" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="149" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7171,7 +7172,7 @@
       </c>
       <c r="H149" s="5"/>
       <c r="I149" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="150" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -7196,7 +7197,7 @@
         <v>454</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7221,7 +7222,7 @@
         <v>458</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7244,7 +7245,7 @@
       </c>
       <c r="H152" s="5"/>
       <c r="I152" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="153" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7269,7 +7270,7 @@
         <v>465</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7292,7 +7293,7 @@
       </c>
       <c r="H154" s="5"/>
       <c r="I154" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -7315,7 +7316,7 @@
       </c>
       <c r="H155" s="5"/>
       <c r="I155" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="156" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7338,7 +7339,7 @@
       </c>
       <c r="H156" s="5"/>
       <c r="I156" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="157" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7361,7 +7362,7 @@
       </c>
       <c r="H157" s="5"/>
       <c r="I157" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="158" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7388,7 +7389,7 @@
         <v>482</v>
       </c>
       <c r="I158" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -7413,7 +7414,7 @@
         <v>486</v>
       </c>
       <c r="I159" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7436,7 +7437,7 @@
       </c>
       <c r="H160" s="5"/>
       <c r="I160" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -7459,7 +7460,7 @@
       </c>
       <c r="H161" s="5"/>
       <c r="I161" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -7482,7 +7483,7 @@
       </c>
       <c r="H162" s="5"/>
       <c r="I162" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7505,7 +7506,7 @@
       </c>
       <c r="H163" s="5"/>
       <c r="I163" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7530,7 +7531,7 @@
         <v>496</v>
       </c>
       <c r="I164" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -7553,7 +7554,7 @@
       </c>
       <c r="H165" s="3"/>
       <c r="I165" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7576,7 +7577,7 @@
       </c>
       <c r="H166" s="5"/>
       <c r="I166" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="167" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7599,7 +7600,7 @@
       </c>
       <c r="H167" s="5"/>
       <c r="I167" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="168" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7622,7 +7623,7 @@
       </c>
       <c r="H168" s="5"/>
       <c r="I168" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7645,7 +7646,7 @@
       </c>
       <c r="H169" s="5"/>
       <c r="I169" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="170" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7668,7 +7669,7 @@
       </c>
       <c r="H170" s="13"/>
       <c r="I170" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -7691,7 +7692,7 @@
       </c>
       <c r="H171" s="13"/>
       <c r="I171" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="172" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -7714,7 +7715,7 @@
       </c>
       <c r="H172" s="13"/>
       <c r="I172" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7736,7 +7737,7 @@
         <v>1</v>
       </c>
       <c r="I173" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="174" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7759,7 +7760,7 @@
       </c>
       <c r="H174" s="8"/>
       <c r="I174" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="175" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7782,7 +7783,7 @@
       </c>
       <c r="H175" s="5"/>
       <c r="I175" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="176" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -7805,7 +7806,7 @@
       </c>
       <c r="H176" s="5"/>
       <c r="I176" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="177" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7828,7 +7829,7 @@
       </c>
       <c r="H177" s="5"/>
       <c r="I177" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="178" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -7851,7 +7852,7 @@
       </c>
       <c r="H178" s="5"/>
       <c r="I178" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="179" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7874,7 +7875,7 @@
       </c>
       <c r="H179" s="8"/>
       <c r="I179" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="180" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7897,7 +7898,7 @@
       </c>
       <c r="H180" s="8"/>
       <c r="I180" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="181" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7920,7 +7921,7 @@
       </c>
       <c r="H181" s="8"/>
       <c r="I181" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7943,7 +7944,7 @@
       </c>
       <c r="H182" s="5"/>
       <c r="I182" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="183" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7966,7 +7967,7 @@
       </c>
       <c r="H183" s="5"/>
       <c r="I183" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="184" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -7989,7 +7990,7 @@
       </c>
       <c r="H184" s="5"/>
       <c r="I184" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8012,7 +8013,7 @@
       </c>
       <c r="H185" s="5"/>
       <c r="I185" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="186" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8035,7 +8036,7 @@
       </c>
       <c r="H186" s="5"/>
       <c r="I186" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="187" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8058,7 +8059,7 @@
       </c>
       <c r="H187" s="5"/>
       <c r="I187" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="188" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8081,7 +8082,7 @@
       </c>
       <c r="H188" s="8"/>
       <c r="I188" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="189" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8104,7 +8105,7 @@
       </c>
       <c r="H189" s="8"/>
       <c r="I189" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="190" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -8127,7 +8128,7 @@
       </c>
       <c r="H190" s="5"/>
       <c r="I190" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="191" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8150,7 +8151,7 @@
       </c>
       <c r="H191" s="5"/>
       <c r="I191" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="192" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8173,7 +8174,7 @@
       </c>
       <c r="H192" s="5"/>
       <c r="I192" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="193" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -8196,7 +8197,7 @@
       </c>
       <c r="H193" s="5"/>
       <c r="I193" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="194" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -8219,7 +8220,7 @@
       </c>
       <c r="H194" s="5"/>
       <c r="I194" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="195" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8242,7 +8243,7 @@
       </c>
       <c r="H195" s="5"/>
       <c r="I195" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="196" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8265,7 +8266,7 @@
       </c>
       <c r="H196" s="13"/>
       <c r="I196" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="197" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8288,7 +8289,7 @@
       </c>
       <c r="H197" s="13"/>
       <c r="I197" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="198" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8311,7 +8312,7 @@
       </c>
       <c r="H198" s="13"/>
       <c r="I198" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="199" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -8334,7 +8335,7 @@
       </c>
       <c r="H199" s="13"/>
       <c r="I199" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="200" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -8357,7 +8358,7 @@
       </c>
       <c r="H200" s="13"/>
       <c r="I200" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="201" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8380,7 +8381,7 @@
       </c>
       <c r="H201" s="13"/>
       <c r="I201" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="202" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8403,7 +8404,7 @@
       </c>
       <c r="H202" s="13"/>
       <c r="I202" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="203" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8426,7 +8427,7 @@
       </c>
       <c r="H203" s="13"/>
       <c r="I203" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="204" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -8449,7 +8450,7 @@
       </c>
       <c r="H204" s="13"/>
       <c r="I204" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="205" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -8472,7 +8473,7 @@
       </c>
       <c r="H205" s="13"/>
       <c r="I205" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="206" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -8495,7 +8496,7 @@
       </c>
       <c r="H206" s="13"/>
       <c r="I206" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="207" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8518,7 +8519,7 @@
       </c>
       <c r="H207" s="13"/>
       <c r="I207" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="208" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8541,7 +8542,7 @@
       </c>
       <c r="H208" s="13"/>
       <c r="I208" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="209" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -8564,7 +8565,7 @@
       </c>
       <c r="H209" s="13"/>
       <c r="I209" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="210" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8587,7 +8588,7 @@
       </c>
       <c r="H210" s="13"/>
       <c r="I210" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="211" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -8610,7 +8611,7 @@
       </c>
       <c r="H211" s="13"/>
       <c r="I211" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="212" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8633,7 +8634,7 @@
       </c>
       <c r="H212" s="13"/>
       <c r="I212" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="213" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8656,7 +8657,7 @@
       </c>
       <c r="H213" s="8"/>
       <c r="I213" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="214" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8679,7 +8680,7 @@
       </c>
       <c r="H214" s="8"/>
       <c r="I214" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="215" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8702,7 +8703,7 @@
       </c>
       <c r="H215" s="8"/>
       <c r="I215" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="216" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -8725,7 +8726,7 @@
       </c>
       <c r="H216" s="5"/>
       <c r="I216" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="217" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8748,7 +8749,7 @@
       </c>
       <c r="H217" s="5"/>
       <c r="I217" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="218" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -8771,7 +8772,7 @@
       </c>
       <c r="H218" s="5"/>
       <c r="I218" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="219" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8794,7 +8795,7 @@
       </c>
       <c r="H219" s="5"/>
       <c r="I219" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="220" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8817,7 +8818,7 @@
       </c>
       <c r="H220" s="8"/>
       <c r="I220" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="221" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8840,7 +8841,7 @@
       </c>
       <c r="H221" s="8"/>
       <c r="I221" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="222" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8863,7 +8864,7 @@
       </c>
       <c r="H222" s="5"/>
       <c r="I222" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="223" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -8888,7 +8889,7 @@
       </c>
       <c r="H223" s="5"/>
       <c r="I223" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="224" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -8911,7 +8912,7 @@
       </c>
       <c r="H224" s="5"/>
       <c r="I224" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="225" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8936,7 +8937,7 @@
       </c>
       <c r="H225" s="5"/>
       <c r="I225" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="226" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8961,7 +8962,7 @@
       </c>
       <c r="H226" s="5"/>
       <c r="I226" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="227" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8984,7 +8985,7 @@
       </c>
       <c r="H227" s="5"/>
       <c r="I227" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="228" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -9009,7 +9010,7 @@
       </c>
       <c r="H228" s="5"/>
       <c r="I228" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="229" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -9032,7 +9033,7 @@
       </c>
       <c r="H229" s="5"/>
       <c r="I229" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="230" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -9057,7 +9058,7 @@
       </c>
       <c r="H230" s="5"/>
       <c r="I230" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="231" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -9080,7 +9081,7 @@
       </c>
       <c r="H231" s="5"/>
       <c r="I231" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="232" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -9103,7 +9104,7 @@
       </c>
       <c r="H232" s="5"/>
       <c r="I232" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="233" spans="1:9" ht="118" x14ac:dyDescent="0.2">
@@ -9128,7 +9129,7 @@
       </c>
       <c r="H233" s="5"/>
       <c r="I233" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="234" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -9151,7 +9152,7 @@
       </c>
       <c r="H234" s="5"/>
       <c r="I234" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="235" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -9174,7 +9175,7 @@
       </c>
       <c r="H235" s="5"/>
       <c r="I235" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="236" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -9199,7 +9200,7 @@
       </c>
       <c r="H236" s="5"/>
       <c r="I236" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="237" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9222,7 +9223,7 @@
       </c>
       <c r="H237" s="5"/>
       <c r="I237" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="238" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -9245,7 +9246,7 @@
       </c>
       <c r="H238" s="5"/>
       <c r="I238" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="239" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -9265,7 +9266,7 @@
         <v>1</v>
       </c>
       <c r="I239" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="240" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -9288,7 +9289,7 @@
       </c>
       <c r="H240" s="13"/>
       <c r="I240" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="241" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -9311,7 +9312,7 @@
       </c>
       <c r="H241" s="13"/>
       <c r="I241" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="242" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -9334,7 +9335,7 @@
       </c>
       <c r="H242" s="8"/>
       <c r="I242" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="243" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9357,7 +9358,7 @@
       </c>
       <c r="H243" s="5"/>
       <c r="I243" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="244" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9380,7 +9381,7 @@
       </c>
       <c r="H244" s="5"/>
       <c r="I244" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="245" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -9403,7 +9404,7 @@
       </c>
       <c r="H245" s="5"/>
       <c r="I245" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="246" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -9426,7 +9427,7 @@
       </c>
       <c r="H246" s="5"/>
       <c r="I246" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="247" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9449,7 +9450,7 @@
       </c>
       <c r="H247" s="5"/>
       <c r="I247" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="248" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -9472,7 +9473,7 @@
       </c>
       <c r="H248" s="5"/>
       <c r="I248" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="249" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -9495,7 +9496,7 @@
       </c>
       <c r="H249" s="5"/>
       <c r="I249" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="250" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -9518,7 +9519,7 @@
       </c>
       <c r="H250" s="5"/>
       <c r="I250" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="251" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9541,7 +9542,7 @@
       </c>
       <c r="H251" s="5"/>
       <c r="I251" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="252" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -9564,7 +9565,7 @@
       </c>
       <c r="H252" s="5"/>
       <c r="I252" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="253" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9587,7 +9588,7 @@
       </c>
       <c r="H253" s="5"/>
       <c r="I253" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="254" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -9610,7 +9611,7 @@
       </c>
       <c r="H254" s="5"/>
       <c r="I254" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="255" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -9633,7 +9634,7 @@
       </c>
       <c r="H255" s="5"/>
       <c r="I255" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="256" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -9656,7 +9657,7 @@
       </c>
       <c r="H256" s="5"/>
       <c r="I256" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="257" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9679,7 +9680,7 @@
       </c>
       <c r="H257" s="5"/>
       <c r="I257" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="258" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -9699,7 +9700,7 @@
         <v>2</v>
       </c>
       <c r="I258" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="259" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -9722,7 +9723,7 @@
       </c>
       <c r="H259" s="5"/>
       <c r="I259" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="260" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -9745,7 +9746,7 @@
       </c>
       <c r="H260" s="5"/>
       <c r="I260" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="261" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -9768,7 +9769,7 @@
       </c>
       <c r="H261" s="5"/>
       <c r="I261" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="262" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -9793,7 +9794,7 @@
         <v>351</v>
       </c>
       <c r="I262" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="263" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9818,7 +9819,7 @@
         <v>783</v>
       </c>
       <c r="I263" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="264" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -9843,7 +9844,7 @@
         <v>787</v>
       </c>
       <c r="I264" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="265" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -9866,7 +9867,7 @@
       </c>
       <c r="H265" s="5"/>
       <c r="I265" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="266" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -9889,7 +9890,7 @@
       </c>
       <c r="H266" s="5"/>
       <c r="I266" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="267" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9912,7 +9913,7 @@
       </c>
       <c r="H267" s="5"/>
       <c r="I267" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="268" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -9937,7 +9938,7 @@
         <v>351</v>
       </c>
       <c r="I268" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="269" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -9962,7 +9963,7 @@
         <v>221</v>
       </c>
       <c r="I269" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="270" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -9987,7 +9988,7 @@
         <v>23</v>
       </c>
       <c r="I270" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="271" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -10012,7 +10013,7 @@
         <v>803</v>
       </c>
       <c r="I271" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="272" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10037,7 +10038,7 @@
         <v>806</v>
       </c>
       <c r="I272" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="273" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -10060,7 +10061,7 @@
       </c>
       <c r="H273" s="5"/>
       <c r="I273" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="274" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -10083,7 +10084,7 @@
       </c>
       <c r="H274" s="3"/>
       <c r="I274" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="275" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -10106,7 +10107,7 @@
       </c>
       <c r="H275" s="3"/>
       <c r="I275" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="276" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10129,7 +10130,7 @@
       </c>
       <c r="H276" s="3"/>
       <c r="I276" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="277" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -10152,7 +10153,7 @@
       </c>
       <c r="H277" s="8"/>
       <c r="I277" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="278" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10175,7 +10176,7 @@
       </c>
       <c r="H278" s="5"/>
       <c r="I278" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="279" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -10198,7 +10199,7 @@
       </c>
       <c r="H279" s="5"/>
       <c r="I279" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="280" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10221,7 +10222,7 @@
       </c>
       <c r="H280" s="5"/>
       <c r="I280" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="281" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -10244,7 +10245,7 @@
       </c>
       <c r="H281" s="5"/>
       <c r="I281" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="282" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10267,7 +10268,7 @@
       </c>
       <c r="H282" s="5"/>
       <c r="I282" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="283" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -10290,7 +10291,7 @@
       </c>
       <c r="H283" s="5"/>
       <c r="I283" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="284" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -10313,7 +10314,7 @@
       </c>
       <c r="H284" s="5"/>
       <c r="I284" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="285" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10327,511 +10328,511 @@
         <v>28479</v>
       </c>
       <c r="F285" s="5" t="s">
-        <v>844</v>
+        <v>1070</v>
       </c>
       <c r="G285" s="7" t="s">
         <v>203</v>
       </c>
       <c r="I285" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="286" spans="1:9" ht="79" x14ac:dyDescent="0.2">
       <c r="A286" s="5" t="s">
+        <v>844</v>
+      </c>
+      <c r="B286" s="5" t="s">
         <v>845</v>
       </c>
-      <c r="B286" s="5" t="s">
+      <c r="C286" s="5" t="s">
         <v>846</v>
-      </c>
-      <c r="C286" s="5" t="s">
-        <v>847</v>
       </c>
       <c r="D286" s="5"/>
       <c r="E286" s="5"/>
       <c r="F286" s="5" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="G286" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H286" s="8"/>
       <c r="I286" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="287" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A287" s="5" t="s">
+        <v>848</v>
+      </c>
+      <c r="B287" s="5" t="s">
+        <v>845</v>
+      </c>
+      <c r="C287" s="5" t="s">
         <v>849</v>
-      </c>
-      <c r="B287" s="5" t="s">
-        <v>846</v>
-      </c>
-      <c r="C287" s="5" t="s">
-        <v>850</v>
       </c>
       <c r="D287" s="5"/>
       <c r="E287" s="5"/>
       <c r="F287" s="5" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="G287" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H287" s="8"/>
       <c r="I287" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="288" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A288" s="5" t="s">
+        <v>851</v>
+      </c>
+      <c r="B288" s="5" t="s">
+        <v>845</v>
+      </c>
+      <c r="C288" s="5" t="s">
         <v>852</v>
-      </c>
-      <c r="B288" s="5" t="s">
-        <v>846</v>
-      </c>
-      <c r="C288" s="5" t="s">
-        <v>853</v>
       </c>
       <c r="D288" s="5"/>
       <c r="E288" s="5"/>
       <c r="F288" s="5" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G288" s="7" t="s">
         <v>50</v>
       </c>
       <c r="H288" s="8"/>
       <c r="I288" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="289" spans="1:9" ht="27" x14ac:dyDescent="0.2">
       <c r="A289" s="5" t="s">
+        <v>854</v>
+      </c>
+      <c r="B289" s="5" t="s">
+        <v>845</v>
+      </c>
+      <c r="C289" s="5" t="s">
         <v>855</v>
-      </c>
-      <c r="B289" s="5" t="s">
-        <v>846</v>
-      </c>
-      <c r="C289" s="5" t="s">
-        <v>856</v>
       </c>
       <c r="D289" s="5"/>
       <c r="E289" s="5"/>
       <c r="F289" s="5" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="G289" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H289" s="5"/>
       <c r="I289" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="290" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A290" s="5" t="s">
+        <v>857</v>
+      </c>
+      <c r="B290" s="5" t="s">
         <v>858</v>
       </c>
-      <c r="B290" s="5" t="s">
+      <c r="C290" s="15" t="s">
         <v>859</v>
-      </c>
-      <c r="C290" s="15" t="s">
-        <v>860</v>
       </c>
       <c r="D290" s="5"/>
       <c r="E290" s="5"/>
       <c r="F290" s="5" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G290" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H290" s="8"/>
       <c r="I290" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="291" spans="1:9" ht="105" x14ac:dyDescent="0.2">
       <c r="A291" s="5" t="s">
+        <v>861</v>
+      </c>
+      <c r="B291" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="C291" s="15" t="s">
         <v>862</v>
-      </c>
-      <c r="B291" s="5" t="s">
-        <v>859</v>
-      </c>
-      <c r="C291" s="15" t="s">
-        <v>863</v>
       </c>
       <c r="D291" s="5"/>
       <c r="E291" s="5"/>
       <c r="F291" s="5" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="G291" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H291" s="5"/>
       <c r="I291" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="292" spans="1:9" ht="66" x14ac:dyDescent="0.2">
       <c r="A292" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="B292" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="C292" s="15" t="s">
         <v>865</v>
-      </c>
-      <c r="B292" s="5" t="s">
-        <v>859</v>
-      </c>
-      <c r="C292" s="15" t="s">
-        <v>866</v>
       </c>
       <c r="D292" s="5"/>
       <c r="E292" s="5"/>
       <c r="F292" s="5" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="G292" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H292" s="5"/>
       <c r="I292" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="293" spans="1:9" ht="27" x14ac:dyDescent="0.2">
       <c r="A293" s="5" t="s">
+        <v>867</v>
+      </c>
+      <c r="B293" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="C293" s="15" t="s">
         <v>868</v>
-      </c>
-      <c r="B293" s="5" t="s">
-        <v>859</v>
-      </c>
-      <c r="C293" s="15" t="s">
-        <v>869</v>
       </c>
       <c r="D293" s="5"/>
       <c r="E293" s="5"/>
       <c r="F293" s="5" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="G293" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H293" s="5"/>
       <c r="I293" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="294" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A294" s="5" t="s">
+        <v>870</v>
+      </c>
+      <c r="B294" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="C294" s="15" t="s">
         <v>871</v>
-      </c>
-      <c r="B294" s="5" t="s">
-        <v>859</v>
-      </c>
-      <c r="C294" s="15" t="s">
-        <v>872</v>
       </c>
       <c r="D294" s="5"/>
       <c r="E294" s="5"/>
       <c r="F294" s="5" t="s">
+        <v>872</v>
+      </c>
+      <c r="G294" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H294" s="5" t="s">
         <v>873</v>
       </c>
-      <c r="G294" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H294" s="5" t="s">
-        <v>874</v>
-      </c>
       <c r="I294" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="295" spans="1:9" ht="27" x14ac:dyDescent="0.2">
       <c r="A295" s="5" t="s">
+        <v>874</v>
+      </c>
+      <c r="B295" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="C295" s="15" t="s">
         <v>875</v>
-      </c>
-      <c r="B295" s="5" t="s">
-        <v>859</v>
-      </c>
-      <c r="C295" s="15" t="s">
-        <v>876</v>
       </c>
       <c r="D295" s="5"/>
       <c r="E295" s="5"/>
       <c r="F295" s="5" t="s">
+        <v>876</v>
+      </c>
+      <c r="G295" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H295" s="5" t="s">
         <v>877</v>
       </c>
-      <c r="G295" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H295" s="5" t="s">
-        <v>878</v>
-      </c>
       <c r="I295" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="296" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A296" s="5" t="s">
+        <v>878</v>
+      </c>
+      <c r="B296" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="C296" s="15" t="s">
         <v>879</v>
-      </c>
-      <c r="B296" s="5" t="s">
-        <v>859</v>
-      </c>
-      <c r="C296" s="15" t="s">
-        <v>880</v>
       </c>
       <c r="D296" s="5"/>
       <c r="E296" s="5"/>
       <c r="F296" s="5" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G296" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H296" s="5"/>
       <c r="I296" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="297" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A297" s="5" t="s">
+        <v>881</v>
+      </c>
+      <c r="B297" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="C297" s="15" t="s">
         <v>882</v>
-      </c>
-      <c r="B297" s="5" t="s">
-        <v>859</v>
-      </c>
-      <c r="C297" s="15" t="s">
-        <v>883</v>
       </c>
       <c r="D297" s="5"/>
       <c r="E297" s="5"/>
       <c r="F297" s="5" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="G297" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H297" s="5"/>
       <c r="I297" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="298" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A298" s="5" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B298" s="5" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C298" s="16">
         <v>1931</v>
       </c>
       <c r="F298" s="5" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="G298" s="7">
         <v>1</v>
       </c>
       <c r="H298" s="5" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="I298" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="299" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A299" s="5" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B299" s="5" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C299" s="9">
         <v>14016</v>
       </c>
       <c r="F299" s="5" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="G299" s="7">
         <v>1</v>
       </c>
       <c r="H299" s="5" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="I299" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="300" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A300" s="5" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B300" s="5" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C300" s="9">
         <v>14388</v>
       </c>
       <c r="F300" s="5" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="G300" s="7">
         <v>1</v>
       </c>
       <c r="H300" s="5" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="I300" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="301" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A301" s="5" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="B301" s="5" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C301" s="9">
         <v>14542</v>
       </c>
       <c r="F301" s="5" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="G301" s="7">
         <v>2</v>
       </c>
       <c r="H301" s="5" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="I301" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="302" spans="1:9" ht="66" x14ac:dyDescent="0.2">
       <c r="A302" s="5" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B302" s="5" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C302" s="9">
         <v>14562</v>
       </c>
       <c r="F302" s="5" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G302" s="7">
         <v>2</v>
       </c>
       <c r="I302" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="303" spans="1:9" ht="27" x14ac:dyDescent="0.2">
       <c r="A303" s="5" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B303" s="5" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C303" s="9">
         <v>15012</v>
       </c>
       <c r="F303" s="5" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="G303" s="7">
         <v>1</v>
       </c>
       <c r="H303" s="5" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="I303" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="304" spans="1:9" ht="27" x14ac:dyDescent="0.2">
       <c r="A304" s="5" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B304" s="5" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C304" s="9">
         <v>15012</v>
       </c>
       <c r="F304" s="5" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="G304" s="7">
         <v>1</v>
       </c>
       <c r="H304" s="5" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="I304" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="305" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A305" s="5" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="B305" s="5" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C305" s="9">
         <v>15304</v>
       </c>
       <c r="F305" s="5" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="G305" s="7">
         <v>2</v>
       </c>
       <c r="H305" s="5" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="I305" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="306" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A306" s="5" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B306" s="5" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C306" s="9">
         <v>15318</v>
       </c>
       <c r="F306" s="5" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="G306" s="7">
         <v>1</v>
       </c>
       <c r="H306" s="5" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="I306" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="307" spans="1:9" ht="66" x14ac:dyDescent="0.2">
       <c r="A307" s="5" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B307" s="5" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C307" s="9">
         <v>17047</v>
       </c>
       <c r="F307" s="5" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="G307" s="7">
         <v>1</v>
@@ -10840,794 +10841,794 @@
         <v>465</v>
       </c>
       <c r="I307" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="308" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A308" s="5" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B308" s="5" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C308" s="9">
         <v>17299</v>
       </c>
       <c r="F308" s="5" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="G308" s="7">
         <v>1</v>
       </c>
       <c r="H308" s="5" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="I308" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="309" spans="1:9" ht="27" x14ac:dyDescent="0.2">
       <c r="A309" s="5" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B309" s="5" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C309" s="9">
         <v>18244</v>
       </c>
       <c r="F309" s="5" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="G309" s="7">
         <v>1</v>
       </c>
       <c r="H309" s="5" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="I309" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="310" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A310" s="5" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B310" s="5" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C310" s="9">
         <v>19142</v>
       </c>
       <c r="F310" s="5" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="G310" s="7">
         <v>1</v>
       </c>
       <c r="I310" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="311" spans="1:9" ht="27" x14ac:dyDescent="0.2">
       <c r="A311" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="B311" s="5" t="s">
         <v>920</v>
       </c>
-      <c r="B311" s="5" t="s">
+      <c r="C311" s="5" t="s">
         <v>921</v>
-      </c>
-      <c r="C311" s="5" t="s">
-        <v>922</v>
       </c>
       <c r="D311" s="5"/>
       <c r="E311" s="5"/>
       <c r="F311" s="5" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="G311" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H311" s="8"/>
       <c r="I311" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="312" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A312" s="5" t="s">
+        <v>923</v>
+      </c>
+      <c r="B312" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="C312" s="5" t="s">
         <v>924</v>
-      </c>
-      <c r="B312" s="5" t="s">
-        <v>921</v>
-      </c>
-      <c r="C312" s="5" t="s">
-        <v>925</v>
       </c>
       <c r="D312" s="5"/>
       <c r="E312" s="5"/>
       <c r="F312" s="5" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="G312" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H312" s="5"/>
       <c r="I312" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="313" spans="1:9" ht="79" x14ac:dyDescent="0.2">
       <c r="A313" s="5" t="s">
+        <v>926</v>
+      </c>
+      <c r="B313" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="C313" s="5" t="s">
         <v>927</v>
-      </c>
-      <c r="B313" s="5" t="s">
-        <v>921</v>
-      </c>
-      <c r="C313" s="5" t="s">
-        <v>928</v>
       </c>
       <c r="D313" s="5"/>
       <c r="E313" s="5"/>
       <c r="F313" s="5" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="G313" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H313" s="5"/>
       <c r="I313" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="314" spans="1:9" ht="66" x14ac:dyDescent="0.2">
       <c r="A314" s="5" t="s">
+        <v>929</v>
+      </c>
+      <c r="B314" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="C314" s="5" t="s">
         <v>930</v>
-      </c>
-      <c r="B314" s="5" t="s">
-        <v>921</v>
-      </c>
-      <c r="C314" s="5" t="s">
-        <v>931</v>
       </c>
       <c r="D314" s="5"/>
       <c r="E314" s="5"/>
       <c r="F314" s="5" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="G314" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H314" s="5"/>
       <c r="I314" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="315" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A315" s="5" t="s">
+        <v>932</v>
+      </c>
+      <c r="B315" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="C315" s="5" t="s">
         <v>933</v>
-      </c>
-      <c r="B315" s="5" t="s">
-        <v>921</v>
-      </c>
-      <c r="C315" s="5" t="s">
-        <v>934</v>
       </c>
       <c r="D315" s="5"/>
       <c r="E315" s="5"/>
       <c r="F315" s="5" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="G315" s="7" t="s">
         <v>120</v>
       </c>
       <c r="H315" s="5"/>
       <c r="I315" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="316" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A316" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="B316" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="C316" s="5" t="s">
         <v>936</v>
-      </c>
-      <c r="B316" s="5" t="s">
-        <v>921</v>
-      </c>
-      <c r="C316" s="5" t="s">
-        <v>937</v>
       </c>
       <c r="D316" s="5"/>
       <c r="E316" s="5"/>
       <c r="F316" s="5" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="G316" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H316" s="5"/>
       <c r="I316" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="317" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A317" s="5" t="s">
+        <v>938</v>
+      </c>
+      <c r="B317" s="5" t="s">
         <v>939</v>
       </c>
-      <c r="B317" s="5" t="s">
+      <c r="C317" s="5" t="s">
         <v>940</v>
-      </c>
-      <c r="C317" s="5" t="s">
-        <v>941</v>
       </c>
       <c r="D317" s="5"/>
       <c r="E317" s="5"/>
       <c r="F317" s="5" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="G317" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H317" s="8"/>
       <c r="I317" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="318" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A318" s="5" t="s">
+        <v>942</v>
+      </c>
+      <c r="B318" s="5" t="s">
+        <v>939</v>
+      </c>
+      <c r="C318" s="5" t="s">
         <v>943</v>
-      </c>
-      <c r="B318" s="5" t="s">
-        <v>940</v>
-      </c>
-      <c r="C318" s="5" t="s">
-        <v>944</v>
       </c>
       <c r="D318" s="5"/>
       <c r="E318" s="5"/>
       <c r="F318" s="5" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="G318" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H318" s="5"/>
       <c r="I318" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="319" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A319" s="5" t="s">
+        <v>945</v>
+      </c>
+      <c r="B319" s="5" t="s">
+        <v>939</v>
+      </c>
+      <c r="C319" s="5" t="s">
         <v>946</v>
-      </c>
-      <c r="B319" s="5" t="s">
-        <v>940</v>
-      </c>
-      <c r="C319" s="5" t="s">
-        <v>947</v>
       </c>
       <c r="D319" s="5"/>
       <c r="E319" s="5"/>
       <c r="F319" s="5" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="G319" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H319" s="5"/>
       <c r="I319" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="320" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A320" s="5" t="s">
+        <v>948</v>
+      </c>
+      <c r="B320" s="5" t="s">
+        <v>939</v>
+      </c>
+      <c r="C320" s="5" t="s">
         <v>949</v>
-      </c>
-      <c r="B320" s="5" t="s">
-        <v>940</v>
-      </c>
-      <c r="C320" s="5" t="s">
-        <v>950</v>
       </c>
       <c r="D320" s="5"/>
       <c r="E320" s="5"/>
       <c r="F320" s="5" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="G320" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H320" s="5"/>
       <c r="I320" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="321" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A321" s="5" t="s">
+        <v>951</v>
+      </c>
+      <c r="B321" s="5" t="s">
+        <v>939</v>
+      </c>
+      <c r="C321" s="5" t="s">
         <v>952</v>
-      </c>
-      <c r="B321" s="5" t="s">
-        <v>940</v>
-      </c>
-      <c r="C321" s="5" t="s">
-        <v>953</v>
       </c>
       <c r="D321" s="5"/>
       <c r="E321" s="5"/>
       <c r="F321" s="5" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G321" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H321" s="5"/>
       <c r="I321" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="322" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A322" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="B322" s="5" t="s">
         <v>955</v>
       </c>
-      <c r="B322" s="5" t="s">
+      <c r="C322" s="5" t="s">
         <v>956</v>
-      </c>
-      <c r="C322" s="5" t="s">
-        <v>957</v>
       </c>
       <c r="D322" s="5"/>
       <c r="E322" s="5"/>
       <c r="F322" s="5" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G322" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H322" s="8"/>
       <c r="I322" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="323" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A323" s="5" t="s">
+        <v>958</v>
+      </c>
+      <c r="B323" s="5" t="s">
+        <v>955</v>
+      </c>
+      <c r="C323" s="5" t="s">
         <v>959</v>
-      </c>
-      <c r="B323" s="5" t="s">
-        <v>956</v>
-      </c>
-      <c r="C323" s="5" t="s">
-        <v>960</v>
       </c>
       <c r="D323" s="5"/>
       <c r="E323" s="5"/>
       <c r="F323" s="5" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G323" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H323" s="5"/>
       <c r="I323" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="324" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A324" s="5" t="s">
+        <v>961</v>
+      </c>
+      <c r="B324" s="5" t="s">
+        <v>955</v>
+      </c>
+      <c r="C324" s="5" t="s">
         <v>962</v>
-      </c>
-      <c r="B324" s="5" t="s">
-        <v>956</v>
-      </c>
-      <c r="C324" s="5" t="s">
-        <v>963</v>
       </c>
       <c r="D324" s="5"/>
       <c r="E324" s="5"/>
       <c r="F324" s="5" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="G324" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H324" s="5"/>
       <c r="I324" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="325" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A325" s="5" t="s">
+        <v>964</v>
+      </c>
+      <c r="B325" s="5" t="s">
+        <v>955</v>
+      </c>
+      <c r="C325" s="5" t="s">
         <v>965</v>
-      </c>
-      <c r="B325" s="5" t="s">
-        <v>956</v>
-      </c>
-      <c r="C325" s="5" t="s">
-        <v>966</v>
       </c>
       <c r="D325" s="5"/>
       <c r="E325" s="5"/>
       <c r="F325" s="5" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="G325" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H325" s="5"/>
       <c r="I325" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="326" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A326" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B326" s="5" t="s">
+        <v>955</v>
+      </c>
+      <c r="C326" s="5" t="s">
         <v>968</v>
-      </c>
-      <c r="B326" s="5" t="s">
-        <v>956</v>
-      </c>
-      <c r="C326" s="5" t="s">
-        <v>969</v>
       </c>
       <c r="D326" s="5"/>
       <c r="E326" s="5"/>
       <c r="F326" s="5" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="G326" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H326" s="5"/>
       <c r="I326" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="327" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A327" s="5" t="s">
+        <v>970</v>
+      </c>
+      <c r="B327" s="5" t="s">
+        <v>955</v>
+      </c>
+      <c r="C327" s="5" t="s">
         <v>971</v>
-      </c>
-      <c r="B327" s="5" t="s">
-        <v>956</v>
-      </c>
-      <c r="C327" s="5" t="s">
-        <v>972</v>
       </c>
       <c r="D327" s="5"/>
       <c r="E327" s="5"/>
       <c r="F327" s="5" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="G327" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H327" s="5"/>
       <c r="I327" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="328" spans="1:9" ht="66" x14ac:dyDescent="0.2">
       <c r="A328" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B328" s="5" t="s">
+        <v>955</v>
+      </c>
+      <c r="C328" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B328" s="5" t="s">
-        <v>956</v>
-      </c>
-      <c r="C328" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="D328" s="5"/>
       <c r="E328" s="5"/>
       <c r="F328" s="5" t="s">
+        <v>975</v>
+      </c>
+      <c r="G328" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H328" s="5" t="s">
         <v>976</v>
       </c>
-      <c r="G328" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H328" s="5" t="s">
-        <v>977</v>
-      </c>
       <c r="I328" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="329" spans="1:9" ht="66" x14ac:dyDescent="0.2">
       <c r="A329" s="5" t="s">
+        <v>977</v>
+      </c>
+      <c r="B329" s="5" t="s">
+        <v>955</v>
+      </c>
+      <c r="C329" s="5" t="s">
         <v>978</v>
-      </c>
-      <c r="B329" s="5" t="s">
-        <v>956</v>
-      </c>
-      <c r="C329" s="5" t="s">
-        <v>979</v>
       </c>
       <c r="D329" s="5"/>
       <c r="E329" s="5"/>
       <c r="F329" s="5" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="G329" s="7" t="s">
         <v>120</v>
       </c>
       <c r="H329" s="5"/>
       <c r="I329" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="330" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A330" s="5" t="s">
+        <v>980</v>
+      </c>
+      <c r="B330" s="5" t="s">
+        <v>955</v>
+      </c>
+      <c r="C330" s="5" t="s">
         <v>981</v>
-      </c>
-      <c r="B330" s="5" t="s">
-        <v>956</v>
-      </c>
-      <c r="C330" s="5" t="s">
-        <v>982</v>
       </c>
       <c r="D330" s="5"/>
       <c r="E330" s="5"/>
       <c r="F330" s="5" t="s">
+        <v>982</v>
+      </c>
+      <c r="G330" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H330" s="5" t="s">
         <v>983</v>
       </c>
-      <c r="G330" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H330" s="5" t="s">
-        <v>984</v>
-      </c>
       <c r="I330" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="331" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A331" s="5" t="s">
+        <v>984</v>
+      </c>
+      <c r="B331" s="5" t="s">
+        <v>955</v>
+      </c>
+      <c r="C331" s="15" t="s">
         <v>985</v>
-      </c>
-      <c r="B331" s="5" t="s">
-        <v>956</v>
-      </c>
-      <c r="C331" s="15" t="s">
-        <v>986</v>
       </c>
       <c r="D331" s="5"/>
       <c r="E331" s="5"/>
       <c r="F331" s="5" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="G331" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H331" s="5" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="I331" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="332" spans="1:9" ht="66" x14ac:dyDescent="0.2">
       <c r="A332" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="B332" s="5" t="s">
+        <v>955</v>
+      </c>
+      <c r="C332" s="15" t="s">
         <v>989</v>
-      </c>
-      <c r="B332" s="5" t="s">
-        <v>956</v>
-      </c>
-      <c r="C332" s="15" t="s">
-        <v>990</v>
       </c>
       <c r="D332" s="5"/>
       <c r="E332" s="5"/>
       <c r="F332" s="5" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="G332" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H332" s="5"/>
       <c r="I332" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="333" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A333" s="5" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B333" s="5" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C333" s="9">
         <v>14798</v>
       </c>
       <c r="F333" s="5" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="G333" s="7">
         <v>1</v>
       </c>
       <c r="H333" s="5" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="I333" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="334" spans="1:9" ht="66" x14ac:dyDescent="0.2">
       <c r="A334" s="5" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B334" s="5" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C334" s="9">
         <v>20354</v>
       </c>
       <c r="F334" s="5" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="G334" s="7">
         <v>2</v>
       </c>
       <c r="H334" s="5" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="I334" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="335" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A335" s="5" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B335" s="5" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C335" s="9">
         <v>22737</v>
       </c>
       <c r="F335" s="5" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="G335" s="7">
         <v>1</v>
       </c>
       <c r="I335" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="336" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A336" s="5" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="B336" s="5" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C336" s="9">
         <v>22923</v>
       </c>
       <c r="F336" s="5" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="G336" s="7">
         <v>2</v>
       </c>
       <c r="I336" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="337" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A337" s="5" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B337" s="5" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C337" s="9">
         <v>25457</v>
       </c>
       <c r="F337" s="5" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="G337" s="7">
         <v>2</v>
       </c>
       <c r="I337" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="338" spans="1:9" ht="79" x14ac:dyDescent="0.2">
       <c r="A338" s="5" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B338" s="5" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C338" s="9">
         <v>27210</v>
       </c>
       <c r="F338" s="5" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="G338" s="7">
         <v>1</v>
       </c>
       <c r="I338" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="339" spans="1:9" ht="66" x14ac:dyDescent="0.2">
       <c r="A339" s="5" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B339" s="5" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C339" s="9">
         <v>29124</v>
       </c>
       <c r="F339" s="5" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="G339" s="7">
         <v>2</v>
       </c>
       <c r="H339" s="1" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="I339" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="340" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A340" s="13" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B340" s="13" t="s">
         <v>1009</v>
       </c>
-      <c r="B340" s="13" t="s">
+      <c r="C340" s="13" t="s">
         <v>1010</v>
-      </c>
-      <c r="C340" s="13" t="s">
-        <v>1011</v>
       </c>
       <c r="D340" s="13"/>
       <c r="E340" s="13" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F340" s="5" t="s">
         <v>1012</v>
-      </c>
-      <c r="F340" s="5" t="s">
-        <v>1013</v>
       </c>
       <c r="G340" s="13">
         <v>0</v>
       </c>
       <c r="H340" s="13"/>
       <c r="I340" s="1" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="341" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A341" s="13" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B341" s="13" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C341" s="16" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D341" s="16" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E341" s="9">
         <v>36526</v>
       </c>
       <c r="F341" s="5" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="G341" s="13">
         <v>0</v>
       </c>
       <c r="H341" s="13"/>
       <c r="I341" s="1" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="342" spans="1:9" ht="53" x14ac:dyDescent="0.2">
       <c r="A342" s="13" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B342" s="13" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C342" s="9">
         <v>36268</v>
@@ -11637,22 +11638,22 @@
       </c>
       <c r="E342" s="13"/>
       <c r="F342" s="5" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="G342" s="13">
         <v>0</v>
       </c>
       <c r="H342" s="13"/>
       <c r="I342" s="1" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="343" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A343" s="13" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B343" s="13" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C343" s="9">
         <v>2901</v>
@@ -11662,22 +11663,22 @@
       </c>
       <c r="E343" s="13"/>
       <c r="F343" s="5" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="G343" s="13">
         <v>0</v>
       </c>
       <c r="H343" s="13"/>
       <c r="I343" s="1" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="344" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A344" s="13" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B344" s="13" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C344" s="9">
         <v>13870</v>
@@ -11687,68 +11688,68 @@
       </c>
       <c r="E344" s="13"/>
       <c r="F344" s="5" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="G344" s="13">
         <v>0</v>
       </c>
       <c r="H344" s="13"/>
       <c r="I344" s="1" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="345" spans="1:9" ht="66" x14ac:dyDescent="0.2">
       <c r="A345" s="13" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B345" s="13" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C345" s="16" t="s">
         <v>1022</v>
-      </c>
-      <c r="B345" s="13" t="s">
-        <v>1010</v>
-      </c>
-      <c r="C345" s="16" t="s">
-        <v>1023</v>
       </c>
       <c r="D345" s="16"/>
       <c r="E345" s="13"/>
       <c r="F345" s="5" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="G345" s="13">
         <v>0</v>
       </c>
       <c r="H345" s="13"/>
       <c r="I345" s="1" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="346" spans="1:9" ht="66" x14ac:dyDescent="0.2">
       <c r="A346" s="13" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B346" s="13" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C346" s="16" t="s">
         <v>1025</v>
-      </c>
-      <c r="B346" s="13" t="s">
-        <v>1010</v>
-      </c>
-      <c r="C346" s="16" t="s">
-        <v>1026</v>
       </c>
       <c r="D346" s="16"/>
       <c r="E346" s="13"/>
       <c r="F346" s="5" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="G346" s="13">
         <v>0</v>
       </c>
       <c r="H346" s="13"/>
       <c r="I346" s="1" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="347" spans="1:9" ht="79" x14ac:dyDescent="0.2">
       <c r="A347" s="13" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B347" s="13" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C347" s="9">
         <v>16056</v>
@@ -11760,193 +11761,193 @@
         <v>39083</v>
       </c>
       <c r="F347" s="5" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="G347" s="13">
         <v>0</v>
       </c>
       <c r="H347" s="13"/>
       <c r="I347" s="1" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="348" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A348" s="1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C348" s="9">
         <v>8567</v>
       </c>
       <c r="F348" s="5" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="G348" s="1">
         <v>0</v>
       </c>
       <c r="I348" s="1" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="349" spans="1:9" ht="105" x14ac:dyDescent="0.2">
       <c r="A349" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B349" s="5" t="s">
         <v>1032</v>
-      </c>
-      <c r="B349" s="5" t="s">
-        <v>1033</v>
       </c>
       <c r="C349" s="9">
         <v>13682</v>
       </c>
       <c r="F349" s="5" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="G349" s="1">
         <v>0</v>
       </c>
       <c r="I349" s="1" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="350" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A350" s="1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B350" s="5" t="s">
         <v>1035</v>
-      </c>
-      <c r="B350" s="5" t="s">
-        <v>1036</v>
       </c>
       <c r="C350" s="9">
         <v>20481</v>
       </c>
       <c r="F350" s="5" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="G350" s="1">
         <v>0</v>
       </c>
       <c r="I350" s="1" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="351" spans="1:9" ht="92" x14ac:dyDescent="0.2">
       <c r="A351" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B351" s="5" t="s">
         <v>1038</v>
-      </c>
-      <c r="B351" s="5" t="s">
-        <v>1039</v>
       </c>
       <c r="C351" s="9">
         <v>21613</v>
       </c>
       <c r="F351" s="5" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="G351" s="1">
         <v>0</v>
       </c>
       <c r="I351" s="1" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="352" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A352" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="C352" s="9">
         <v>22266</v>
       </c>
       <c r="F352" s="5" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="G352" s="1">
         <v>0</v>
       </c>
       <c r="I352" s="1" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="353" spans="1:9" ht="79" x14ac:dyDescent="0.2">
       <c r="A353" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B353" s="5" t="s">
         <v>1043</v>
-      </c>
-      <c r="B353" s="5" t="s">
-        <v>1044</v>
       </c>
       <c r="C353" s="9">
         <v>23336</v>
       </c>
       <c r="F353" s="5" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="G353" s="1">
         <v>0</v>
       </c>
       <c r="I353" s="1" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="354" spans="1:9" ht="157" x14ac:dyDescent="0.2">
       <c r="A354" s="1" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="C354" s="9">
         <v>23503</v>
       </c>
       <c r="F354" s="5" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="G354" s="1">
         <v>0</v>
       </c>
       <c r="I354" s="1" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="355" spans="1:9" ht="183" x14ac:dyDescent="0.2">
       <c r="A355" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B355" s="5" t="s">
         <v>1048</v>
-      </c>
-      <c r="B355" s="5" t="s">
-        <v>1049</v>
       </c>
       <c r="C355" s="9">
         <v>27564</v>
       </c>
       <c r="F355" s="5" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="G355" s="1">
         <v>0</v>
       </c>
       <c r="I355" s="1" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="356" spans="1:9" ht="92" x14ac:dyDescent="0.2">
       <c r="A356" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B356" s="5" t="s">
         <v>1051</v>
-      </c>
-      <c r="B356" s="5" t="s">
-        <v>1052</v>
       </c>
       <c r="C356" s="9">
         <v>30977</v>
       </c>
       <c r="F356" s="5" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="G356" s="1">
         <v>0</v>
       </c>
       <c r="I356" s="1" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="357" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A357" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B357" s="1" t="s">
         <v>1054</v>
-      </c>
-      <c r="B357" s="1" t="s">
-        <v>1055</v>
       </c>
       <c r="C357" s="9">
         <v>18023</v>
@@ -11955,21 +11956,21 @@
         <v>23137</v>
       </c>
       <c r="F357" s="5" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="G357" s="1">
         <v>0</v>
       </c>
       <c r="I357" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="358" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A358" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="C358" s="9">
         <v>18571</v>
@@ -11978,13 +11979,13 @@
         <v>27361</v>
       </c>
       <c r="F358" s="5" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="G358" s="1">
         <v>0</v>
       </c>
       <c r="I358" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
   </sheetData>

</xml_diff>